<commit_message>
Update IP - EX 54 - Graficos avancados (Anexo).xlsx
Explicação realizada
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 54 - Graficos avancados (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 54 - Graficos avancados (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A7F011-70ED-4F01-BDCA-60BBF92B5498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929F6D98-F40F-48BA-B455-3CD79D3EBF6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -996,6 +1018,823 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>EXPLICAÇÃO!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Venda</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>EXPLICAÇÃO!$B$11:$C$18</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="8"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>jan</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>jan</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>jan</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>fev</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>fev</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>fev</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>fev</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>joão</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>fernanda</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>thiago</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>maria</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>joão</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>fernanda</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>thiago</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>maria</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EXPLICAÇÃO!$D$11:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>133</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C407-414E-9C82-F7130B2D622C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1515925888"/>
+        <c:axId val="1515934528"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1515925888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515934528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1515934528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515925888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Janeiro</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="76000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>EXPLICAÇÃO!$B$11:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>joão</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>fernanda</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>thiago</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>maria</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>joão</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fernanda</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>thiago</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>maria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EXPLICAÇÃO!$D$11:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-09E6-41E8-9060-FF30AC0371CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Fevereiro</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="77000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-3.2691179044696907E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-09E6-41E8-9060-FF30AC0371CE}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>EXPLICAÇÃO!$B$11:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>joão</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>fernanda</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>thiago</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>maria</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>joão</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>fernanda</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>thiago</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>maria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>EXPLICAÇÃO!$D$15:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>133</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-09E6-41E8-9060-FF30AC0371CE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1515932608"/>
+        <c:axId val="1515933568"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1515932608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515933568"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1515933568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1515932608"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1446,7 +2285,1059 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2042,6 +3933,78 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2A6FE7E-A67A-D598-29CE-1A7A2A962BB8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBB755DB-A457-EAD7-A889-78CB02930683}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2723,8 +4686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,8 +4908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:T36"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3231,7 +5194,10 @@
       <c r="O16" s="47">
         <v>12</v>
       </c>
-      <c r="P16" s="23"/>
+      <c r="P16" s="23" t="e" cm="1">
+        <f t="array" ref="P16">subto</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="76"/>

</xml_diff>